<commit_message>
Fixed Use Case List
</commit_message>
<xml_diff>
--- a/TechDoc/Use Case List.xlsx
+++ b/TechDoc/Use Case List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared\Documents\WorkLectures\Системы программирования\Studentswork\pm-17\yakutcement\TechDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F129E5-7966-40B0-AAF4-08C45A67C4D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599C5AFA-0E24-42E3-806C-04A9E054B77B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,9 +49,6 @@
     <t>Редактировать пользователя</t>
   </si>
   <si>
-    <t>Удалить пользователя</t>
-  </si>
-  <si>
     <t>Изменить справочную информацию</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>Удалить товар</t>
+  </si>
+  <si>
+    <t>Удалить пользователя+список пользователей</t>
   </si>
 </sst>
 </file>
@@ -642,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -664,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -672,10 +672,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -683,10 +683,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,7 +694,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7"/>
     </row>
@@ -703,7 +703,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8"/>
     </row>
@@ -712,7 +712,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9"/>
     </row>
@@ -721,7 +721,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10"/>
     </row>
@@ -730,7 +730,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11"/>
     </row>
@@ -739,7 +739,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -747,7 +747,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -755,7 +755,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -771,7 +771,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -803,7 +803,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -819,7 +819,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -827,7 +827,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -843,7 +843,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -907,10 +907,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -918,10 +918,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -929,10 +929,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -940,10 +940,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -951,10 +951,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,10 +962,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -973,10 +973,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -984,10 +984,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -995,10 +995,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1006,10 +1006,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,10 +1017,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1028,10 +1028,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1039,10 +1039,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1050,10 +1050,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1061,10 +1061,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
         <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1072,10 +1072,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1083,10 +1083,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1094,10 +1094,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed Use Case list
</commit_message>
<xml_diff>
--- a/TechDoc/Use Case List.xlsx
+++ b/TechDoc/Use Case List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared\Documents\WorkLectures\Системы программирования\Studentswork\pm-17\yakutcement\TechDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599C5AFA-0E24-42E3-806C-04A9E054B77B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E758216-269A-4E3F-8DE5-A7999251C3E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>№</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>Удалить пользователя+список пользователей</t>
+  </si>
+  <si>
+    <t>Эвертов Владимир Васильевич</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -641,8 +644,8 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>63</v>
+      <c r="C2" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,7 +699,9 @@
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7"/>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">

</xml_diff>

<commit_message>
Changes in Use case list
</commit_message>
<xml_diff>
--- a/TechDoc/Use Case List.xlsx
+++ b/TechDoc/Use Case List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Shared\Documents\WorkLectures\Системы программирования\Studentswork\pm-17\yakutcement\TechDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C2DAF9-69A9-47CD-82D1-B7A1B5459CDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8648D585-D82B-4C10-A5D5-D94F6B37D0D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>№</t>
   </si>
@@ -265,7 +265,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +275,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -291,11 +297,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -613,7 +620,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -638,7 +645,7 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -668,7 +675,7 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C5" t="s">
@@ -713,7 +720,9 @@
       <c r="B9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C9"/>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">

</xml_diff>